<commit_message>
working containers and sites parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -110,19 +110,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eg. AB, CD</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -235,19 +222,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eg. AB, CD</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -360,19 +334,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eg. AB, CD</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -500,25 +461,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eg. AB, CD</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>Stock</t>
   </si>
@@ -548,9 +496,6 @@
   </si>
   <si>
     <t>Destination</t>
-  </si>
-  <si>
-    <t>Crew</t>
   </si>
   <si>
     <t>End Trough</t>
@@ -979,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J3"/>
+  <dimension ref="A3:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,10 +935,10 @@
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1013,16 +958,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1034,10 +976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K3"/>
+  <dimension ref="A3:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,11 +989,10 @@
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1071,19 +1012,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1095,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K3"/>
+  <dimension ref="A3:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,10 +1046,10 @@
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1131,19 +1069,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1155,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R3"/>
+  <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,10 +1109,10 @@
     <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1120,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1214,31 +1149,28 @@
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update comment handling in parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
     <sheet name="Picking" sheetId="2" r:id="rId2"/>
     <sheet name="Shocking" sheetId="4" r:id="rId3"/>
-    <sheet name="HU Transfer" sheetId="3" r:id="rId4"/>
+    <sheet name="Allocations" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -978,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add event comments to reports
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Shocking" sheetId="4" r:id="rId3"/>
     <sheet name="Allocations" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,24 +172,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If filled, the trough column must also be filled.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -205,11 +204,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Eg. Match the column header to count code selected in app. Use as many columns as needed.  Value should be the counts.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
+          <t>Can be either a drawer (eg. 4.3) or a cup (eg. 4.3.1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Eg. Mandatory set equal to cross if needed.</t>
+          <t>If filled, the trough column must also be filled.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -418,11 +427,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Can be either a drawer (eg. 4.3) or a cup (eg. 4.3.1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Eg. EQU, Bonell, Odell, etc.</t>
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -435,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="O3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +488,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Stock</t>
   </si>
@@ -526,13 +548,28 @@
   </si>
   <si>
     <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Start Container</t>
+  </si>
+  <si>
+    <t>Cleaning Loss</t>
+  </si>
+  <si>
+    <t>Shock Loss</t>
+  </si>
+  <si>
+    <t>Shocking (Y/N)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +589,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -629,12 +672,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,6 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +974,7 @@
   <dimension ref="A3:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,23 +1023,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J3"/>
+  <dimension ref="A2:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1006,25 +1061,37 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1036,7 +1103,7 @@
   <dimension ref="A3:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,37 +1157,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q3"/>
+  <dimension ref="A2:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K2" s="5" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="L2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1134,48 +1206,52 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K2:N2"/>
+  <mergeCells count="2">
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add option to record picks from multiple days in picks parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -220,6 +220,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="L3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Day picks were made</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -440,13 +453,13 @@
     <t>Start Container</t>
   </si>
   <si>
-    <t>Cleaning Loss</t>
-  </si>
-  <si>
-    <t>Shock Loss</t>
-  </si>
-  <si>
     <t>Shocking (Y/N)</t>
+  </si>
+  <si>
+    <t>PICK CODE</t>
+  </si>
+  <si>
+    <t>Cleaning Losses</t>
   </si>
 </sst>
 </file>
@@ -900,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M4"/>
+  <dimension ref="A2:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,20 +924,23 @@
     <col min="3" max="3" width="5.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="8" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
       <c r="I2" s="5"/>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -950,20 +966,32 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1">
+        <v>4</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M4" s="6"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add flexiblity to ED parser date selection
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
     <sheet name="Picking" sheetId="2" r:id="rId2"/>
     <sheet name="Allocations" sheetId="3" r:id="rId3"/>
+    <sheet name="Temperatures" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -387,8 +388,57 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Stock</t>
   </si>
@@ -460,6 +510,12 @@
   </si>
   <si>
     <t>Cleaning Losses</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Temperature(C)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -581,6 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,7 +921,7 @@
   <dimension ref="A3:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,10 +946,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -915,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,4 +1162,47 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
start/end dates on reports, better errors on picks parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -221,19 +221,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Day picks were made</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -438,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>Stock</t>
   </si>
@@ -500,22 +487,25 @@
     <t>Container</t>
   </si>
   <si>
+    <t>Shocking (Y/N)</t>
+  </si>
+  <si>
+    <t>PICK CODE</t>
+  </si>
+  <si>
     <t>Start Container</t>
   </si>
   <si>
-    <t>Shocking (Y/N)</t>
-  </si>
-  <si>
-    <t>PICK CODE</t>
-  </si>
-  <si>
-    <t>Cleaning Losses</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
     <t>Temperature(C)</t>
+  </si>
+  <si>
+    <t>First Hatch Observed (Y/N)</t>
+  </si>
+  <si>
+    <t>100% Hatch Observed (Y/N)</t>
   </si>
 </sst>
 </file>
@@ -618,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -627,7 +617,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -637,7 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,18 +909,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I3"/>
+  <dimension ref="A3:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -959,6 +949,30 @@
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -970,34 +984,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P4"/>
+  <dimension ref="A2:M6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="8" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F2" s="7" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="5"/>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1023,32 +1034,26 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3</v>
-      </c>
-      <c r="O3" s="1">
-        <v>4</v>
-      </c>
-      <c r="P3" s="1">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L4" s="6"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1064,38 +1069,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="L2" s="7" t="s">
+      <c r="F2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="L2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -1155,8 +1155,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="L2:O2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1168,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,17 +1188,17 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="10"/>
+      <c r="D4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add programs to picks and spawning parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg_development.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Program of pairing set in spawning. Optional, must match code in db.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -425,7 +438,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Stock</t>
   </si>
@@ -909,20 +922,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I6"/>
+  <dimension ref="A3:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -936,43 +949,22 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>